<commit_message>
Toma el numero del test plan actualizacion
</commit_message>
<xml_diff>
--- a/build/resources/test/datadriven/DataTestPlan.xlsx
+++ b/build/resources/test/datadriven/DataTestPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scastaño\Bancolombia projects\Automation_Certification\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D207E046-B6F2-42EC-B036-66D6CCA7BA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE952DE-D047-44FD-AEC8-CE282752E963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{7B30B265-8E50-43EC-9686-BAB7CCCE9E11}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="194">
   <si>
     <t>columnId</t>
   </si>
@@ -339,12 +339,6 @@
   </si>
   <si>
     <t>cybersecurityHu</t>
-  </si>
-  <si>
-    <t>AW1003001</t>
-  </si>
-  <si>
-    <t>CDH</t>
   </si>
   <si>
     <t>EVC - DATOS ANALITICA E IA</t>
@@ -590,9 +584,6 @@
     <t>Evidencias VSTS</t>
   </si>
   <si>
-    <t>Automático DevOps</t>
-  </si>
-  <si>
     <t>http://wikiti/wikiti/index.php/CapacidadesAnaliticas-DT</t>
   </si>
   <si>
@@ -638,9 +629,6 @@
     <t>Buenos días, la historia de usuario certificada y debidamente gestionada para coordinar en el paso a producción es la siguiente:</t>
   </si>
   <si>
-    <t>Se devuelve HU a debidamente certificada para su paso a PDN</t>
-  </si>
-  <si>
     <t>Santiago Venegas Zarate</t>
   </si>
   <si>
@@ -665,47 +653,95 @@
     <t>Lista Pipelines</t>
   </si>
   <si>
+    <t>AW1003001_BigDataCompany</t>
+  </si>
+  <si>
+    <t>#4544378</t>
+  </si>
+  <si>
+    <t>#HUParent</t>
+  </si>
+  <si>
+    <t>Certi</t>
+  </si>
+  <si>
+    <t>Las pruebas ejecutadas para este paso a producción fueron ejecutadas manualmente y las evidencias se encuentran en el stage "Stage Manual Test"</t>
+  </si>
+  <si>
+    <t>MANUAL STEP EXECUTION UAT</t>
+  </si>
+  <si>
+    <t>tittleDOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deploymentTool </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pipeline </t>
+  </si>
+  <si>
+    <t>artifact</t>
+  </si>
+  <si>
+    <t>documentation</t>
+  </si>
+  <si>
+    <t>Julio Roberto Suarez Flechas</t>
+  </si>
+  <si>
+    <t>Se devuelve HU  debidamente certificada para su paso a PDN</t>
+  </si>
+  <si>
+    <t>directDataChanges</t>
+  </si>
+  <si>
+    <t>specializedTest</t>
+  </si>
+  <si>
+    <t>solutionDocumentation</t>
+  </si>
+  <si>
+    <t>Automatico DevOps</t>
+  </si>
+  <si>
+    <t>Angel Camilo Calderon Ardila</t>
+  </si>
+  <si>
+    <t>Lincoln Ernesto Perez Perez</t>
+  </si>
+  <si>
+    <t>NU0044001_ProductizarLaAnalitica_MR_ms_LCTopeGastos</t>
+  </si>
+  <si>
+    <t>DAIA 16 - DATACORE</t>
+  </si>
+  <si>
+    <t>NU0044001</t>
+  </si>
+  <si>
+    <t>Productizar LZ Cloud</t>
+  </si>
+  <si>
     <t>NU0044001_ProductizarLaAnalitica</t>
   </si>
   <si>
-    <t>AW1003001_BigDataCompany</t>
-  </si>
-  <si>
-    <t>NU0044001_ProductizarLaAnalitica_MR_ms_ModevaEstimadorIngresos</t>
-  </si>
-  <si>
-    <t>#4544378</t>
-  </si>
-  <si>
-    <t>#HUParent</t>
-  </si>
-  <si>
-    <t>Certi</t>
-  </si>
-  <si>
-    <t>DAIA 14 - FIX IT</t>
+    <t>Habilitador 4834625: Ejecucion movimiento masivo de objetos a historicas, batch operation y delete de objetos Sprint 181</t>
+  </si>
+  <si>
+    <t>Ejecucion movimiento masivo de objetos a historicas</t>
+  </si>
+  <si>
+    <t>trunk.20231218.1</t>
   </si>
   <si>
     <t>Ingestión</t>
-  </si>
-  <si>
-    <t>NU0044001_ProductizarLaAnalitica_MR_ms_PerfilTransaccionalGestionFraude</t>
-  </si>
-  <si>
-    <t>trunk.20231013.1</t>
-  </si>
-  <si>
-    <t>TORRE DE CONTROL - Ingestion Fuente Nueva en la LZ tierra kudu - Celula CCRED10</t>
-  </si>
-  <si>
-    <t>User Story 4613236: (Ronal Gomez Mejia - Equipo Analitica ) TORRE DE CONTROL - Ingestion Fuente Nueva en la LZ tierra kudu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -770,13 +806,26 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -861,7 +910,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1250,19 +1299,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1305,7 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -1386,7 +1422,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1398,33 +1433,19 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1438,23 +1459,47 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1476,12 +1521,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1530,16 +1569,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1857,34 +1893,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE2A0CF-B568-4517-B159-B91ECF8077CE}">
-  <dimension ref="A1:AF72"/>
+  <dimension ref="A1:AN75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="71" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" customWidth="1"/>
     <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.5703125" customWidth="1"/>
-    <col min="12" max="12" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" customWidth="1"/>
-    <col min="14" max="14" width="36.28515625" customWidth="1"/>
-    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" customWidth="1"/>
+    <col min="20" max="20" width="5" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" customWidth="1"/>
+    <col min="23" max="23" width="6" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" customWidth="1"/>
+    <col min="28" max="28" width="7.140625" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" customWidth="1"/>
+    <col min="30" max="30" width="7.28515625" customWidth="1"/>
+    <col min="31" max="31" width="6.5703125" customWidth="1"/>
+    <col min="32" max="32" width="6.28515625" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1919,34 +1970,34 @@
         <v>79</v>
       </c>
       <c r="L1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N1" t="s">
         <v>78</v>
       </c>
       <c r="O1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P1" t="s">
         <v>80</v>
       </c>
       <c r="Q1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R1" t="s">
         <v>81</v>
       </c>
       <c r="S1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="T1" t="s">
         <v>82</v>
       </c>
       <c r="U1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="V1" t="s">
         <v>83</v>
@@ -1961,7 +2012,7 @@
         <v>91</v>
       </c>
       <c r="Z1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AA1" t="s">
         <v>92</v>
@@ -1981,14 +2032,38 @@
       <c r="AF1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" s="6" customFormat="1" ht="27.75" customHeight="1">
+      <c r="AG1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" s="6" customFormat="1" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="str">
+      <c r="B2" s="49" t="str">
         <f>CONCATENATE("TEST PLAN EVC00037_",C16," SPRINT ",B16)</f>
-        <v>TEST PLAN EVC00037_4613236 SPRINT 177</v>
+        <v>TEST PLAN EVC00037_4834625 SPRINT 181</v>
       </c>
       <c r="C2" s="6" t="str">
         <f>VLOOKUP(G16,A40:B73,2,FALSE)</f>
@@ -2003,7 +2078,7 @@
         <v>Alcance
 Se valida que los logs estan correctos y no se encuentren errores que desencadenen una falla
 Historia de usuario:
-  HU4613236 | User Story 4613236: (Ronal Gomez Mejia - Equipo Analitica ) TORRE DE CONTROL - Ingestion Fuente Nueva en la LZ tierra kudu | AW1003001_BigDataCompany | Release-1228| trunk.20231013.1 | 
+  HU4834625 | Habilitador 4834625: Ejecucion movimiento masivo de objetos a historicas, batch operation y delete de objetos Sprint 181 | NU0044001_ProductizarLaAnalitica | Release-737| trunk.20231218.1 | 
 Lineas impactadas: 
 N/A 
 Equipo de trabajo:
@@ -2027,97 +2102,125 @@
       </c>
       <c r="G2" s="6">
         <f>D16</f>
-        <v>4263042</v>
+        <v>4709069</v>
       </c>
       <c r="H2" s="6">
         <f>C16</f>
-        <v>4613236</v>
+        <v>4834625</v>
       </c>
       <c r="I2" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>95</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N2" s="6" t="str">
         <f>I25</f>
-        <v>Pr_TORRE_DE_CONTROL_-_Ingestion_Fuente_Nueva_en_la_LZ_tierra_kudu_-_Celula_CCRED10</v>
+        <v>Pr_Ejecucion_movimiento_masivo_de_objetos_a_historicas</v>
       </c>
       <c r="O2" s="6" t="str">
         <f>A16</f>
         <v>Ingestión</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="54">
         <f>IF(A16="Rutina",1,1000)</f>
         <v>1000</v>
       </c>
-      <c r="Q2" s="6" t="str">
+      <c r="Q2" s="54" t="str">
         <f>IF(A16="Rutina","Archivos","Registros")</f>
         <v>Registros</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="54">
         <f>IF(A16="Rutina",10,30)</f>
         <v>30</v>
       </c>
-      <c r="S2" s="6" t="str">
+      <c r="S2" s="54" t="str">
         <f>IF(A16="Rutina","Mb","Mb")</f>
         <v>Mb</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="54">
         <f>IF(A16="Rutina",10,30)</f>
         <v>30</v>
       </c>
-      <c r="U2" s="6" t="str">
+      <c r="U2" s="54" t="str">
         <f>IF(A16="Rutina","Minutos","Minutos")</f>
         <v>Minutos</v>
       </c>
-      <c r="V2" s="6">
+      <c r="V2" s="54">
         <v>3</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W2" s="54">
         <v>10</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Y2" s="6" t="s">
         <v>40</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AB2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="AC2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>103</v>
-      </c>
       <c r="AE2" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AF2" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32">
+        <v>98</v>
+      </c>
+      <c r="AG2" s="6" t="str">
+        <f>CONCATENATE("DOD EVC00037 SPRINT ",B16," - ","SALIDA HU",C16)</f>
+        <v>DOD EVC00037 SPRINT 181 - SALIDA HU4834625</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ2" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK2" s="6" t="str">
+        <f>C29</f>
+        <v>Automatico DevOps</v>
+      </c>
+      <c r="AL2" s="6" t="str">
+        <f>F21</f>
+        <v>NU0044001_ProductizarLaAnalitica</v>
+      </c>
+      <c r="AM2" s="6" t="str">
+        <f>E21</f>
+        <v>trunk.20231218.1</v>
+      </c>
+      <c r="AN2" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
     </row>
-    <row r="6" spans="1:32" ht="50.25" customHeight="1">
+    <row r="6" spans="1:40" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
@@ -2125,114 +2228,114 @@
         <v>37</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="G6" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="H6" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="I6" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="89.25" customHeight="1">
+    </row>
+    <row r="7" spans="1:40" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="str">
         <f>E16</f>
-        <v>DAIA 14 - FIX IT</v>
+        <v>DAIA 16 - DATACORE</v>
       </c>
       <c r="B7" s="14" t="str">
         <f>F21</f>
-        <v>AW1003001_BigDataCompany</v>
+        <v>NU0044001_ProductizarLaAnalitica</v>
       </c>
       <c r="C7" s="14">
         <f>C21</f>
-        <v>1228</v>
+        <v>737</v>
       </c>
       <c r="D7" s="14">
         <f>C16</f>
-        <v>4613236</v>
+        <v>4834625</v>
       </c>
       <c r="E7" s="14" t="str">
         <f>A21</f>
-        <v>User Story 4613236: (Ronal Gomez Mejia - Equipo Analitica ) TORRE DE CONTROL - Ingestion Fuente Nueva en la LZ tierra kudu</v>
-      </c>
-      <c r="F7" s="35" t="str">
+        <v>Habilitador 4834625: Ejecucion movimiento masivo de objetos a historicas, batch operation y delete de objetos Sprint 181</v>
+      </c>
+      <c r="F7" s="56" t="str">
         <f>F16</f>
-        <v>Evelin Franco Caballero</v>
-      </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-    </row>
-    <row r="8" spans="1:32" ht="15.75" thickBot="1"/>
-    <row r="9" spans="1:32">
-      <c r="A9" s="70" t="s">
+        <v>Felix Daniel Valderrama Pineda</v>
+      </c>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="71"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="72"/>
-    </row>
-    <row r="10" spans="1:32">
-      <c r="A10" s="15" t="s">
+      <c r="C10" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="D10" s="73"/>
+      <c r="E10" s="72" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="73" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="74"/>
-      <c r="E10" s="73" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10" s="75"/>
-    </row>
-    <row r="11" spans="1:32" ht="41.25" customHeight="1" thickBot="1">
+      <c r="F10" s="74"/>
+    </row>
+    <row r="11" spans="1:40" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="78"/>
-    </row>
-    <row r="12" spans="1:32">
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="77"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
     </row>
-    <row r="13" spans="1:32" ht="15.75" thickBot="1">
+    <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
     </row>
-    <row r="14" spans="1:32">
-      <c r="A14" s="79" t="s">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="81"/>
-    </row>
-    <row r="15" spans="1:32">
-      <c r="A15" s="36" t="s">
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="80"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="17" t="s">
@@ -2242,193 +2345,187 @@
         <v>5</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A16" s="35" t="s">
-        <v>177</v>
-      </c>
-      <c r="B16" s="52">
-        <v>177</v>
-      </c>
-      <c r="C16" s="30">
-        <v>4613236</v>
-      </c>
-      <c r="D16" s="58">
-        <v>4263042</v>
-      </c>
-      <c r="E16" s="53" t="s">
-        <v>176</v>
-      </c>
-      <c r="F16" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="43">
+        <v>181</v>
+      </c>
+      <c r="C16" s="60">
+        <v>4834625</v>
+      </c>
+      <c r="D16" s="61">
+        <v>4709069</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="50" t="str">
+      <c r="H16" s="41" t="str">
         <f>CONCATENATE("Evidencias_EVC00037_HU",C16)</f>
-        <v>Evidencias_EVC00037_HU4613236</v>
+        <v>Evidencias_EVC00037_HU4834625</v>
       </c>
       <c r="I16" s="25" t="str">
         <f>CONCATENATE("Salida a PDN EVC00037_HU",C16)</f>
-        <v>Salida a PDN EVC00037_HU4613236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A19" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66" t="s">
+        <v>Salida a PDN EVC00037_HU4834625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="68"/>
+      <c r="F19" s="36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="43" t="s">
+      <c r="B20" s="27" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="28" t="s">
+      <c r="C20" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="D20" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="E20" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="F20" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="46" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A21" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="C21" s="56">
-        <v>1228</v>
+    </row>
+    <row r="21" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="58" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="53">
+        <v>737</v>
       </c>
       <c r="D21" s="25" t="str">
         <f>CONCATENATE("Release-",C21)</f>
-        <v>Release-1228</v>
-      </c>
-      <c r="E21" s="54" t="s">
-        <v>179</v>
-      </c>
-      <c r="F21" s="60" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="23" spans="1:12" s="36" customFormat="1">
-      <c r="A23" s="87" t="s">
+        <v>Release-737</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="86" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+    </row>
+    <row r="24" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="88"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="38"/>
-    </row>
-    <row r="24" spans="1:12" s="26" customFormat="1">
-      <c r="A24" s="28" t="s">
+      <c r="C24" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" s="84" t="s">
         <v>133</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="I24" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="D24" s="85" t="s">
+      <c r="J24" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="I24" s="26" t="s">
+      <c r="K24" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="J24" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="K24" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="L24" s="39"/>
-    </row>
-    <row r="25" spans="1:12" s="36" customFormat="1" ht="72.75" customHeight="1" thickBot="1">
-      <c r="A25" s="42">
-        <v>4700921</v>
-      </c>
-      <c r="B25" s="24" t="str">
+    </row>
+    <row r="25" spans="1:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="35" t="str">
         <f>CONCATENATE("TEST PLAN EVC00037_",C16," SPRINT ",B16)</f>
-        <v>TEST PLAN EVC00037_4613236 SPRINT 177</v>
-      </c>
-      <c r="C25" s="24" t="s">
+        <v>TEST PLAN EVC00037_4834625 SPRINT 181</v>
+      </c>
+      <c r="C25" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="86" t="str">
+      <c r="D25" s="85" t="str">
         <f>CONCATENATE("HU",C16," | ",A21," | ",F21," | ",D21, "| ",E21," | ")</f>
-        <v xml:space="preserve">HU4613236 | User Story 4613236: (Ronal Gomez Mejia - Equipo Analitica ) TORRE DE CONTROL - Ingestion Fuente Nueva en la LZ tierra kudu | AW1003001_BigDataCompany | Release-1228| trunk.20231013.1 | </v>
-      </c>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="I25" s="40" t="str">
+        <v xml:space="preserve">HU4834625 | Habilitador 4834625: Ejecucion movimiento masivo de objetos a historicas, batch operation y delete de objetos Sprint 181 | NU0044001_ProductizarLaAnalitica | Release-737| trunk.20231218.1 | </v>
+      </c>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="52" t="str">
         <f>CONCATENATE("Pr_",SUBSTITUTE(B21," ","_"),)</f>
-        <v>Pr_TORRE_DE_CONTROL_-_Ingestion_Fuente_Nueva_en_la_LZ_tierra_kudu_-_Celula_CCRED10</v>
-      </c>
-      <c r="J25" s="42">
+        <v>Pr_Ejecucion_movimiento_masivo_de_objetos_a_historicas</v>
+      </c>
+      <c r="J25" s="34">
         <f>D16</f>
-        <v>4263042</v>
-      </c>
-      <c r="K25" s="30">
+        <v>4709069</v>
+      </c>
+      <c r="K25" s="34">
         <v>4544378</v>
       </c>
-      <c r="L25" s="38"/>
-    </row>
-    <row r="26" spans="1:12" ht="45.75" customHeight="1" thickBot="1">
+    </row>
+    <row r="26" spans="1:11" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -2438,127 +2535,133 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A27" s="82" t="s">
-        <v>117</v>
-      </c>
-      <c r="B27" s="83"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="84"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="31" t="s">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="83"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="D28" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="F28" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="32" t="s">
+      <c r="G28" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="F28" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="G28" s="33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="68.25" customHeight="1" thickBot="1">
-      <c r="A29" s="57"/>
+    </row>
+    <row r="29" spans="1:11" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="45"/>
       <c r="B29" s="24" t="str">
         <f>CONCATENATE("DOD EVC00037 SPRINT ",B16," - ","SALIDA HU",C16)</f>
-        <v>DOD EVC00037 SPRINT 177 - SALIDA HU4613236</v>
+        <v>DOD EVC00037 SPRINT 181 - SALIDA HU4834625</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="D29" s="24" t="str">
+        <v>182</v>
+      </c>
+      <c r="D29" s="41" t="str">
         <f>F21</f>
-        <v>AW1003001_BigDataCompany</v>
+        <v>NU0044001_ProductizarLaAnalitica</v>
       </c>
       <c r="E29" s="24" t="str">
         <f>E21</f>
-        <v>trunk.20231013.1</v>
+        <v>trunk.20231218.1</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="G29" s="25" t="str">
+        <v>143</v>
+      </c>
+      <c r="G29" s="55" t="str">
         <f>CONCATENATE("Evidencia VSTS: ",A25)</f>
-        <v>Evidencia VSTS: 4700921</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="31" spans="1:12">
-      <c r="A31" s="68" t="s">
+        <v xml:space="preserve">Evidencia VSTS: </v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="69"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="47" t="s">
+      <c r="B33" s="35" t="str">
+        <f>G29</f>
+        <v xml:space="preserve">Evidencia VSTS: </v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="60.75" thickBot="1">
-      <c r="A33" s="23" t="s">
+      <c r="B36" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="B33" s="25" t="str">
-        <f>G29</f>
-        <v>Evidencia VSTS: 4700921</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="61" t="s">
+      <c r="C36" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="28" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="C37" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30.75" thickBot="1">
-      <c r="A37" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="B37" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>15</v>
       </c>
@@ -2566,10 +2669,10 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>30</v>
       </c>
@@ -2577,10 +2680,10 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -2588,10 +2691,10 @@
         <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>14</v>
       </c>
@@ -2599,10 +2702,10 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>33</v>
       </c>
@@ -2610,32 +2713,26 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
       </c>
-      <c r="C46" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
       </c>
-      <c r="C47" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>19</v>
       </c>
@@ -2643,7 +2740,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -2651,7 +2748,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>31</v>
       </c>
@@ -2659,7 +2756,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -2667,7 +2764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -2675,15 +2772,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>32</v>
       </c>
@@ -2691,7 +2788,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>9</v>
       </c>
@@ -2699,7 +2796,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>24</v>
       </c>
@@ -2707,7 +2804,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>38</v>
       </c>
@@ -2715,7 +2812,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>13</v>
       </c>
@@ -2723,7 +2820,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>39</v>
       </c>
@@ -2731,7 +2828,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>28</v>
       </c>
@@ -2739,7 +2836,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>10</v>
       </c>
@@ -2747,15 +2844,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" t="s">
         <v>147</v>
       </c>
-      <c r="B62" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>18</v>
       </c>
@@ -2763,7 +2860,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>22</v>
       </c>
@@ -2771,7 +2868,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>11</v>
       </c>
@@ -2779,7 +2876,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>40</v>
       </c>
@@ -2787,7 +2884,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>12</v>
       </c>
@@ -2795,7 +2892,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>29</v>
       </c>
@@ -2803,7 +2900,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>23</v>
       </c>
@@ -2811,15 +2908,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="51" t="s">
-        <v>162</v>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="42" t="s">
+        <v>158</v>
       </c>
       <c r="B70" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>74</v>
       </c>
@@ -2827,12 +2924,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B72" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2840,20 +2952,20 @@
     <sortCondition ref="A72"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="D24:G24"/>
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{8DFF09A0-456D-478B-86E4-09A5CEBE87E8}">
@@ -2877,21 +2989,22 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E16" xr:uid="{AA8D74F9-2EB6-46D8-A52C-E708B99E7E27}">
       <formula1>"DAIA 13 - I Y D BIGDATA, DAIA 14 - FIX IT,  DAIA 15 - DRACARYS,DAIA 16 - DATACORE,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7" xr:uid="{18B303FE-EC30-41C9-A61E-455BD9AE514E}">
-      <formula1>$A$41:$A$72</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:G16" xr:uid="{FFDCED8A-6F94-4D6C-8C75-CA3248735151}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G16" xr:uid="{18B303FE-EC30-41C9-A61E-455BD9AE514E}">
       <formula1>$A$41:$A$73</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21" xr:uid="{F62E2613-224E-4BF0-996A-0B4B24AD935D}">
-      <formula1>$C$41:$C$47</formula1>
+      <formula1>$C$41:$C$46</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16 F7" xr:uid="{984ED40C-CC8D-4FDE-A388-3840913BBF3E}">
+      <formula1>$A$41:$A$80</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B65" r:id="rId1" xr:uid="{002EF672-AFCF-4F50-A701-A1B00501F5A8}"/>
     <hyperlink ref="F29" r:id="rId2" xr:uid="{06FF4803-01E1-468B-A2CC-25BA213933AD}"/>
+    <hyperlink ref="AJ2" r:id="rId3" xr:uid="{070A2185-528B-48B7-86B4-9285B5979F85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>